<commit_message>
Call Monitoring Tracking Additional Column
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateCarriedForward.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateCarriedForward.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\udminsure\UDM.Insurance.Interface\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TyronR\Desktop\Source\udminsure\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F21ABA-06AD-4922-BE9A-25A1091CF7F9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870CD631-F0C1-4DA4-AB30-C1F9ACF38014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20520" yWindow="6960" windowWidth="19125" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="54">
   <si>
     <t>TOTALS</t>
   </si>
@@ -191,6 +195,9 @@
   </si>
   <si>
     <t>% Total Saved Carried Forwards</t>
+  </si>
+  <si>
+    <t>% Saved by Call Monitoring Agent</t>
   </si>
 </sst>
 </file>
@@ -473,7 +480,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -653,6 +660,20 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -995,31 +1016,33 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Y21"/>
+  <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:U1"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="6" width="9.5703125" customWidth="1"/>
-    <col min="7" max="13" width="8.42578125" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="8.42578125" customWidth="1"/>
-    <col min="17" max="17" width="10" customWidth="1"/>
-    <col min="18" max="18" width="9" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="8.42578125" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="8.42578125" customWidth="1"/>
-    <col min="21" max="21" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="8.42578125" hidden="1" customWidth="1"/>
-    <col min="24" max="25" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="4" width="8.7265625" customWidth="1"/>
+    <col min="5" max="6" width="9.54296875" customWidth="1"/>
+    <col min="7" max="9" width="8.453125" customWidth="1"/>
+    <col min="10" max="10" width="8.453125" style="96" customWidth="1"/>
+    <col min="11" max="14" width="8.453125" customWidth="1"/>
+    <col min="15" max="15" width="9.1796875" customWidth="1"/>
+    <col min="16" max="16" width="9.1796875" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="8.453125" customWidth="1"/>
+    <col min="18" max="18" width="10" customWidth="1"/>
+    <col min="19" max="19" width="9" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="8.453125" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="8.453125" customWidth="1"/>
+    <col min="22" max="22" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="8.453125" hidden="1" customWidth="1"/>
+    <col min="25" max="26" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="79" t="s">
         <v>33</v>
       </c>
@@ -1042,11 +1065,12 @@
       <c r="R1" s="80"/>
       <c r="S1" s="80"/>
       <c r="T1" s="80"/>
-      <c r="U1" s="81"/>
-      <c r="V1" s="69"/>
-      <c r="W1" s="70"/>
-    </row>
-    <row r="2" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="U1" s="80"/>
+      <c r="V1" s="81"/>
+      <c r="W1" s="69"/>
+      <c r="X1" s="70"/>
+    </row>
+    <row r="2" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="23"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -1056,19 +1080,20 @@
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
+      <c r="J2" s="87"/>
       <c r="K2" s="20"/>
       <c r="L2" s="20"/>
-      <c r="N2" s="21"/>
+      <c r="M2" s="20"/>
       <c r="O2" s="21"/>
       <c r="P2" s="21"/>
       <c r="Q2" s="21"/>
-      <c r="R2" s="20"/>
+      <c r="R2" s="21"/>
       <c r="S2" s="20"/>
-      <c r="T2" s="19"/>
+      <c r="T2" s="20"/>
       <c r="U2" s="19"/>
-    </row>
-    <row r="3" spans="1:25" s="61" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V2" s="19"/>
+    </row>
+    <row r="3" spans="1:26" s="61" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="78"/>
       <c r="B3" s="78"/>
       <c r="C3" s="78"/>
@@ -1092,8 +1117,9 @@
       <c r="U3" s="78"/>
       <c r="V3" s="78"/>
       <c r="W3" s="78"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X3" s="78"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="59"/>
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
@@ -1103,7 +1129,7 @@
       <c r="G4" s="59"/>
       <c r="H4" s="59"/>
       <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
+      <c r="J4" s="88"/>
       <c r="K4" s="59"/>
       <c r="L4" s="59"/>
       <c r="M4" s="59"/>
@@ -1115,8 +1141,9 @@
       <c r="S4" s="59"/>
       <c r="T4" s="59"/>
       <c r="U4" s="59"/>
-    </row>
-    <row r="5" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V4" s="59"/>
+    </row>
+    <row r="5" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="14"/>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
@@ -1126,20 +1153,21 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
+      <c r="J5" s="89"/>
       <c r="K5" s="14"/>
       <c r="L5" s="14"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="16"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="17"/>
       <c r="O5" s="16"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="16"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="14"/>
-    </row>
-    <row r="6" spans="1:25" ht="65.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P5" s="16"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="14"/>
+    </row>
+    <row r="6" spans="1:26" ht="66" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="40" t="s">
         <v>15</v>
       </c>
@@ -1167,52 +1195,55 @@
       <c r="I6" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="42" t="s">
+      <c r="J6" s="90" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="K6" s="42" t="s">
+      <c r="L6" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="L6" s="42" t="s">
+      <c r="M6" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="M6" s="42" t="s">
+      <c r="N6" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="43" t="s">
+      <c r="O6" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="O6" s="42" t="s">
+      <c r="P6" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="P6" s="42" t="s">
+      <c r="Q6" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="Q6" s="44" t="s">
+      <c r="R6" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="R6" s="42" t="s">
+      <c r="S6" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="S6" s="44" t="s">
+      <c r="T6" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="T6" s="42" t="s">
+      <c r="U6" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="U6" s="44" t="s">
+      <c r="V6" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="V6" s="71" t="s">
+      <c r="W6" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="W6" s="42" t="s">
+      <c r="X6" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="X6" s="13"/>
       <c r="Y6" s="13"/>
-    </row>
-    <row r="7" spans="1:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="Z6" s="13"/>
+    </row>
+    <row r="7" spans="1:26" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A7" s="28" t="s">
         <v>1</v>
       </c>
@@ -1233,48 +1264,49 @@
       </c>
       <c r="I7" s="77"/>
       <c r="J7" s="30"/>
-      <c r="K7" s="77"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="32">
+      <c r="K7" s="30"/>
+      <c r="L7" s="77"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="32">
         <v>169</v>
       </c>
-      <c r="N7" s="33">
-        <f>M7/G7</f>
+      <c r="O7" s="33">
+        <f>N7/G7</f>
         <v>0.59507042253521125</v>
       </c>
-      <c r="O7" s="65">
-        <f>N7-M7</f>
+      <c r="P7" s="65">
+        <f>O7-N7</f>
         <v>-168.4049295774648</v>
       </c>
-      <c r="P7" s="35">
+      <c r="Q7" s="35">
         <v>12</v>
       </c>
-      <c r="Q7" s="36">
-        <f>P7/G7</f>
+      <c r="R7" s="36">
+        <f>Q7/G7</f>
         <v>4.2253521126760563E-2</v>
       </c>
-      <c r="R7" s="29">
-        <f>M7+P7</f>
+      <c r="S7" s="29">
+        <f>N7+Q7</f>
         <v>181</v>
       </c>
-      <c r="S7" s="37">
-        <f>R7/G7</f>
+      <c r="T7" s="37">
+        <f>S7/G7</f>
         <v>0.63732394366197187</v>
       </c>
-      <c r="T7" s="38">
-        <f>G7-R7</f>
+      <c r="U7" s="38">
+        <f>G7-S7</f>
         <v>103</v>
       </c>
-      <c r="U7" s="67">
-        <f>T7/G7</f>
+      <c r="V7" s="67">
+        <f>U7/G7</f>
         <v>0.36267605633802819</v>
       </c>
-      <c r="V7" s="66"/>
       <c r="W7" s="66"/>
-      <c r="X7" s="1"/>
+      <c r="X7" s="66"/>
       <c r="Y7" s="1"/>
-    </row>
-    <row r="8" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Z7" s="1"/>
+    </row>
+    <row r="8" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>0</v>
       </c>
@@ -1286,27 +1318,28 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="J8" s="91"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="9">
-        <f>G7-M7</f>
+      <c r="M8" s="2"/>
+      <c r="N8" s="9">
+        <f>G7-N7</f>
         <v>115</v>
       </c>
-      <c r="N8" s="7"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="4"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="1"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="3"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z8" s="1"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -1316,24 +1349,25 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="J9" s="91"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="1"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="3"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z9" s="1"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" s="57"/>
       <c r="B10" s="58"/>
       <c r="C10" s="58"/>
@@ -1343,24 +1377,25 @@
       <c r="G10" s="57"/>
       <c r="H10" s="58"/>
       <c r="I10" s="58"/>
-      <c r="J10" s="58"/>
+      <c r="J10" s="92"/>
       <c r="K10" s="58"/>
       <c r="L10" s="58"/>
       <c r="M10" s="58"/>
-      <c r="N10" s="57"/>
-      <c r="O10" s="58"/>
-      <c r="P10" s="57"/>
-      <c r="Q10" s="58"/>
-      <c r="R10" s="57"/>
-      <c r="S10" s="58"/>
-      <c r="T10" s="57"/>
-      <c r="U10" s="58"/>
-      <c r="V10" s="1"/>
+      <c r="N10" s="58"/>
+      <c r="O10" s="57"/>
+      <c r="P10" s="58"/>
+      <c r="Q10" s="57"/>
+      <c r="R10" s="58"/>
+      <c r="S10" s="57"/>
+      <c r="T10" s="58"/>
+      <c r="U10" s="57"/>
+      <c r="V10" s="58"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z10" s="1"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" s="24"/>
       <c r="B11" s="24"/>
       <c r="C11" s="24"/>
@@ -1370,20 +1405,21 @@
       <c r="G11" s="24"/>
       <c r="H11" s="24"/>
       <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
+      <c r="J11" s="93"/>
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
-      <c r="M11" s="25"/>
+      <c r="M11" s="24"/>
       <c r="N11" s="25"/>
       <c r="O11" s="25"/>
       <c r="P11" s="25"/>
       <c r="Q11" s="25"/>
       <c r="R11" s="25"/>
-      <c r="S11" s="24"/>
+      <c r="S11" s="25"/>
       <c r="T11" s="24"/>
-      <c r="U11" s="11"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="U11" s="24"/>
+      <c r="V11" s="11"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -1393,24 +1429,25 @@
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
+      <c r="J12" s="5"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="3"/>
-      <c r="V12" s="1"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="3"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z12" s="1"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" s="6"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -1420,24 +1457,25 @@
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
+      <c r="J13" s="5"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="3"/>
-      <c r="V13" s="1"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="3"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z13" s="1"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" s="6"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -1447,24 +1485,25 @@
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
+      <c r="J14" s="5"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="4"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="1"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="3"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z14" s="1"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" s="24"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -1474,24 +1513,25 @@
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
+      <c r="J15" s="5"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="4"/>
-      <c r="U15" s="3"/>
-      <c r="V15" s="1"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="3"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z15" s="1"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" s="6"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -1501,24 +1541,25 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
+      <c r="J16" s="5"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="6"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="4"/>
-      <c r="U16" s="3"/>
-      <c r="V16" s="1"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="3"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Z16" s="1"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="26"/>
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
@@ -1528,10 +1569,10 @@
       <c r="G17" s="26"/>
       <c r="H17" s="26"/>
       <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
+      <c r="J17" s="94"/>
       <c r="K17" s="26"/>
       <c r="L17" s="26"/>
-      <c r="M17" s="27"/>
+      <c r="M17" s="26"/>
       <c r="N17" s="27"/>
       <c r="O17" s="27"/>
       <c r="P17" s="27"/>
@@ -1539,8 +1580,9 @@
       <c r="R17" s="27"/>
       <c r="S17" s="27"/>
       <c r="T17" s="27"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U17" s="27"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" s="26"/>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
@@ -1550,10 +1592,10 @@
       <c r="G18" s="26"/>
       <c r="H18" s="26"/>
       <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="J18" s="94"/>
       <c r="K18" s="26"/>
       <c r="L18" s="26"/>
-      <c r="M18" s="27"/>
+      <c r="M18" s="26"/>
       <c r="N18" s="27"/>
       <c r="O18" s="27"/>
       <c r="P18" s="27"/>
@@ -1561,8 +1603,9 @@
       <c r="R18" s="27"/>
       <c r="S18" s="27"/>
       <c r="T18" s="27"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U18" s="27"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" s="27"/>
       <c r="B19" s="27"/>
       <c r="C19" s="27"/>
@@ -1572,7 +1615,7 @@
       <c r="G19" s="27"/>
       <c r="H19" s="27"/>
       <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
+      <c r="J19" s="95"/>
       <c r="K19" s="27"/>
       <c r="L19" s="27"/>
       <c r="M19" s="27"/>
@@ -1583,8 +1626,9 @@
       <c r="R19" s="27"/>
       <c r="S19" s="27"/>
       <c r="T19" s="27"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U19" s="27"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" s="27"/>
       <c r="B20" s="27"/>
       <c r="C20" s="27"/>
@@ -1594,7 +1638,7 @@
       <c r="G20" s="27"/>
       <c r="H20" s="27"/>
       <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
+      <c r="J20" s="95"/>
       <c r="K20" s="27"/>
       <c r="L20" s="27"/>
       <c r="M20" s="27"/>
@@ -1605,8 +1649,9 @@
       <c r="R20" s="27"/>
       <c r="S20" s="27"/>
       <c r="T20" s="27"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U20" s="27"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" s="27"/>
       <c r="B21" s="27"/>
       <c r="C21" s="27"/>
@@ -1616,7 +1661,7 @@
       <c r="G21" s="27"/>
       <c r="H21" s="27"/>
       <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
+      <c r="J21" s="95"/>
       <c r="K21" s="27"/>
       <c r="L21" s="27"/>
       <c r="M21" s="27"/>
@@ -1627,14 +1672,15 @@
       <c r="R21" s="27"/>
       <c r="S21" s="27"/>
       <c r="T21" s="27"/>
+      <c r="U21" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A3:W3"/>
-    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="A3:X3"/>
+    <mergeCell ref="A1:V1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="77" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1643,31 +1689,33 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Y21"/>
+  <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:U1"/>
+    <sheetView view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J4" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="6" width="9.5703125" customWidth="1"/>
-    <col min="7" max="13" width="8.42578125" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="8.42578125" customWidth="1"/>
-    <col min="17" max="17" width="10" customWidth="1"/>
-    <col min="18" max="18" width="9" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="8.42578125" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="8.42578125" customWidth="1"/>
-    <col min="21" max="21" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="8.42578125" hidden="1" customWidth="1"/>
-    <col min="24" max="25" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="4" width="8.7265625" customWidth="1"/>
+    <col min="5" max="6" width="9.54296875" customWidth="1"/>
+    <col min="7" max="9" width="8.453125" customWidth="1"/>
+    <col min="10" max="10" width="8.453125" style="96" customWidth="1"/>
+    <col min="11" max="14" width="8.453125" customWidth="1"/>
+    <col min="15" max="15" width="9.1796875" customWidth="1"/>
+    <col min="16" max="16" width="9.1796875" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="8.453125" customWidth="1"/>
+    <col min="18" max="18" width="10" customWidth="1"/>
+    <col min="19" max="19" width="9" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="8.453125" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="8.453125" customWidth="1"/>
+    <col min="22" max="22" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="8.453125" hidden="1" customWidth="1"/>
+    <col min="25" max="26" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="79" t="s">
         <v>34</v>
       </c>
@@ -1690,11 +1738,12 @@
       <c r="R1" s="80"/>
       <c r="S1" s="80"/>
       <c r="T1" s="80"/>
-      <c r="U1" s="81"/>
-      <c r="V1" s="69"/>
-      <c r="W1" s="70"/>
-    </row>
-    <row r="2" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="U1" s="80"/>
+      <c r="V1" s="81"/>
+      <c r="W1" s="69"/>
+      <c r="X1" s="70"/>
+    </row>
+    <row r="2" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="23"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -1704,19 +1753,20 @@
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
+      <c r="J2" s="87"/>
       <c r="K2" s="20"/>
       <c r="L2" s="20"/>
-      <c r="N2" s="21"/>
+      <c r="M2" s="20"/>
       <c r="O2" s="21"/>
       <c r="P2" s="21"/>
       <c r="Q2" s="21"/>
-      <c r="R2" s="20"/>
+      <c r="R2" s="21"/>
       <c r="S2" s="20"/>
-      <c r="T2" s="19"/>
+      <c r="T2" s="20"/>
       <c r="U2" s="19"/>
-    </row>
-    <row r="3" spans="1:25" s="61" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V2" s="19"/>
+    </row>
+    <row r="3" spans="1:26" s="61" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="78"/>
       <c r="B3" s="78"/>
       <c r="C3" s="78"/>
@@ -1740,8 +1790,9 @@
       <c r="U3" s="78"/>
       <c r="V3" s="78"/>
       <c r="W3" s="78"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X3" s="78"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="59"/>
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
@@ -1751,7 +1802,7 @@
       <c r="G4" s="59"/>
       <c r="H4" s="59"/>
       <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
+      <c r="J4" s="88"/>
       <c r="K4" s="59"/>
       <c r="L4" s="59"/>
       <c r="M4" s="59"/>
@@ -1763,8 +1814,9 @@
       <c r="S4" s="59"/>
       <c r="T4" s="59"/>
       <c r="U4" s="59"/>
-    </row>
-    <row r="5" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V4" s="59"/>
+    </row>
+    <row r="5" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="14"/>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
@@ -1774,20 +1826,21 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
+      <c r="J5" s="89"/>
       <c r="K5" s="14"/>
       <c r="L5" s="14"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="16"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="17"/>
       <c r="O5" s="16"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="16"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="14"/>
-    </row>
-    <row r="6" spans="1:25" ht="65.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P5" s="16"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="14"/>
+    </row>
+    <row r="6" spans="1:26" ht="66" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="40" t="s">
         <v>30</v>
       </c>
@@ -1815,52 +1868,55 @@
       <c r="I6" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="42" t="s">
+      <c r="J6" s="90" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="K6" s="42" t="s">
+      <c r="L6" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="L6" s="42" t="s">
+      <c r="M6" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="M6" s="42" t="s">
+      <c r="N6" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="43" t="s">
+      <c r="O6" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="O6" s="42" t="s">
+      <c r="P6" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="P6" s="42" t="s">
+      <c r="Q6" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="Q6" s="44" t="s">
+      <c r="R6" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="R6" s="42" t="s">
+      <c r="S6" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="S6" s="44" t="s">
+      <c r="T6" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="T6" s="42" t="s">
+      <c r="U6" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="U6" s="44" t="s">
+      <c r="V6" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="V6" s="71" t="s">
+      <c r="W6" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="W6" s="42" t="s">
+      <c r="X6" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="X6" s="13"/>
       <c r="Y6" s="13"/>
-    </row>
-    <row r="7" spans="1:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="Z6" s="13"/>
+    </row>
+    <row r="7" spans="1:26" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A7" s="64"/>
       <c r="B7" s="46">
         <v>12245</v>
@@ -1879,48 +1935,49 @@
       </c>
       <c r="I7" s="77"/>
       <c r="J7" s="30"/>
-      <c r="K7" s="77"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="32">
+      <c r="K7" s="30"/>
+      <c r="L7" s="77"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="32">
         <v>169</v>
       </c>
-      <c r="N7" s="33">
-        <f>M7/G7</f>
+      <c r="O7" s="33">
+        <f>N7/G7</f>
         <v>0.59507042253521125</v>
       </c>
-      <c r="O7" s="65">
-        <f>N7-M7</f>
+      <c r="P7" s="65">
+        <f>O7-N7</f>
         <v>-168.4049295774648</v>
       </c>
-      <c r="P7" s="35">
+      <c r="Q7" s="35">
         <v>12</v>
       </c>
-      <c r="Q7" s="36">
-        <f>P7/G7</f>
+      <c r="R7" s="36">
+        <f>Q7/G7</f>
         <v>4.2253521126760563E-2</v>
       </c>
-      <c r="R7" s="29">
-        <f>M7+P7</f>
+      <c r="S7" s="29">
+        <f>N7+Q7</f>
         <v>181</v>
       </c>
-      <c r="S7" s="37">
-        <f>R7/G7</f>
+      <c r="T7" s="37">
+        <f>S7/G7</f>
         <v>0.63732394366197187</v>
       </c>
-      <c r="T7" s="38">
-        <f>G7-R7</f>
+      <c r="U7" s="38">
+        <f>G7-S7</f>
         <v>103</v>
       </c>
-      <c r="U7" s="67">
-        <f>T7/G7</f>
+      <c r="V7" s="67">
+        <f>U7/G7</f>
         <v>0.36267605633802819</v>
       </c>
-      <c r="V7" s="66"/>
       <c r="W7" s="66"/>
-      <c r="X7" s="1"/>
+      <c r="X7" s="66"/>
       <c r="Y7" s="1"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z7" s="1"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" s="68" t="s">
         <v>38</v>
       </c>
@@ -1941,48 +1998,49 @@
       </c>
       <c r="I8" s="77"/>
       <c r="J8" s="30"/>
-      <c r="K8" s="77"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="32">
+      <c r="K8" s="30"/>
+      <c r="L8" s="77"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="32">
         <v>169</v>
       </c>
-      <c r="N8" s="33">
-        <f>M8/G8</f>
+      <c r="O8" s="33">
+        <f>N8/G8</f>
         <v>0.59507042253521125</v>
       </c>
-      <c r="O8" s="65">
-        <f>N8-M8</f>
+      <c r="P8" s="65">
+        <f>O8-N8</f>
         <v>-168.4049295774648</v>
       </c>
-      <c r="P8" s="35">
+      <c r="Q8" s="35">
         <v>12</v>
       </c>
-      <c r="Q8" s="36">
-        <f>P8/G8</f>
+      <c r="R8" s="36">
+        <f>Q8/G8</f>
         <v>4.2253521126760563E-2</v>
       </c>
-      <c r="R8" s="29">
-        <f>M8+P8</f>
+      <c r="S8" s="29">
+        <f>N8+Q8</f>
         <v>181</v>
       </c>
-      <c r="S8" s="37">
-        <f>R8/G8</f>
+      <c r="T8" s="37">
+        <f>S8/G8</f>
         <v>0.63732394366197187</v>
       </c>
-      <c r="T8" s="38">
-        <f>G8-R8</f>
+      <c r="U8" s="38">
+        <f>G8-S8</f>
         <v>103</v>
       </c>
-      <c r="U8" s="67">
-        <f>T8/G8</f>
+      <c r="V8" s="67">
+        <f>U8/G8</f>
         <v>0.36267605633802819</v>
       </c>
-      <c r="V8" s="66"/>
       <c r="W8" s="66"/>
-      <c r="X8" s="1"/>
+      <c r="X8" s="66"/>
       <c r="Y8" s="1"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z8" s="1"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -1992,24 +2050,25 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="J9" s="91"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="1"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="3"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z9" s="1"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" s="57"/>
       <c r="B10" s="58"/>
       <c r="C10" s="58"/>
@@ -2019,24 +2078,25 @@
       <c r="G10" s="57"/>
       <c r="H10" s="58"/>
       <c r="I10" s="58"/>
-      <c r="J10" s="58"/>
+      <c r="J10" s="92"/>
       <c r="K10" s="58"/>
       <c r="L10" s="58"/>
       <c r="M10" s="58"/>
-      <c r="N10" s="57"/>
-      <c r="O10" s="58"/>
-      <c r="P10" s="57"/>
-      <c r="Q10" s="58"/>
-      <c r="R10" s="57"/>
-      <c r="S10" s="58"/>
-      <c r="T10" s="57"/>
-      <c r="U10" s="58"/>
-      <c r="V10" s="1"/>
+      <c r="N10" s="58"/>
+      <c r="O10" s="57"/>
+      <c r="P10" s="58"/>
+      <c r="Q10" s="57"/>
+      <c r="R10" s="58"/>
+      <c r="S10" s="57"/>
+      <c r="T10" s="58"/>
+      <c r="U10" s="57"/>
+      <c r="V10" s="58"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z10" s="1"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" s="24"/>
       <c r="B11" s="24"/>
       <c r="C11" s="24"/>
@@ -2046,20 +2106,21 @@
       <c r="G11" s="24"/>
       <c r="H11" s="24"/>
       <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
+      <c r="J11" s="93"/>
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
-      <c r="M11" s="25"/>
+      <c r="M11" s="24"/>
       <c r="N11" s="25"/>
       <c r="O11" s="25"/>
       <c r="P11" s="25"/>
       <c r="Q11" s="25"/>
       <c r="R11" s="25"/>
-      <c r="S11" s="24"/>
+      <c r="S11" s="25"/>
       <c r="T11" s="24"/>
-      <c r="U11" s="11"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="U11" s="24"/>
+      <c r="V11" s="11"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -2069,24 +2130,25 @@
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
+      <c r="J12" s="5"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="3"/>
-      <c r="V12" s="1"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="3"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z12" s="1"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" s="6"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -2096,24 +2158,25 @@
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
+      <c r="J13" s="5"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="3"/>
-      <c r="V13" s="1"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="3"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z13" s="1"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" s="6"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -2123,24 +2186,25 @@
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
+      <c r="J14" s="5"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="4"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="1"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="3"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z14" s="1"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" s="24"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -2150,24 +2214,25 @@
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
+      <c r="J15" s="5"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="4"/>
-      <c r="U15" s="3"/>
-      <c r="V15" s="1"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="3"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z15" s="1"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" s="6"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -2177,24 +2242,25 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
+      <c r="J16" s="5"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="6"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="4"/>
-      <c r="U16" s="3"/>
-      <c r="V16" s="1"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="3"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Z16" s="1"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="26"/>
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
@@ -2204,10 +2270,10 @@
       <c r="G17" s="26"/>
       <c r="H17" s="26"/>
       <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
+      <c r="J17" s="94"/>
       <c r="K17" s="26"/>
       <c r="L17" s="26"/>
-      <c r="M17" s="27"/>
+      <c r="M17" s="26"/>
       <c r="N17" s="27"/>
       <c r="O17" s="27"/>
       <c r="P17" s="27"/>
@@ -2215,8 +2281,9 @@
       <c r="R17" s="27"/>
       <c r="S17" s="27"/>
       <c r="T17" s="27"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U17" s="27"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" s="26"/>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
@@ -2226,10 +2293,10 @@
       <c r="G18" s="26"/>
       <c r="H18" s="26"/>
       <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="J18" s="94"/>
       <c r="K18" s="26"/>
       <c r="L18" s="26"/>
-      <c r="M18" s="27"/>
+      <c r="M18" s="26"/>
       <c r="N18" s="27"/>
       <c r="O18" s="27"/>
       <c r="P18" s="27"/>
@@ -2237,8 +2304,9 @@
       <c r="R18" s="27"/>
       <c r="S18" s="27"/>
       <c r="T18" s="27"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U18" s="27"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" s="27"/>
       <c r="B19" s="27"/>
       <c r="C19" s="27"/>
@@ -2248,7 +2316,7 @@
       <c r="G19" s="27"/>
       <c r="H19" s="27"/>
       <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
+      <c r="J19" s="95"/>
       <c r="K19" s="27"/>
       <c r="L19" s="27"/>
       <c r="M19" s="27"/>
@@ -2259,8 +2327,9 @@
       <c r="R19" s="27"/>
       <c r="S19" s="27"/>
       <c r="T19" s="27"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U19" s="27"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" s="27"/>
       <c r="B20" s="27"/>
       <c r="C20" s="27"/>
@@ -2270,7 +2339,7 @@
       <c r="G20" s="27"/>
       <c r="H20" s="27"/>
       <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
+      <c r="J20" s="95"/>
       <c r="K20" s="27"/>
       <c r="L20" s="27"/>
       <c r="M20" s="27"/>
@@ -2281,8 +2350,9 @@
       <c r="R20" s="27"/>
       <c r="S20" s="27"/>
       <c r="T20" s="27"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U20" s="27"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" s="27"/>
       <c r="B21" s="27"/>
       <c r="C21" s="27"/>
@@ -2292,7 +2362,7 @@
       <c r="G21" s="27"/>
       <c r="H21" s="27"/>
       <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
+      <c r="J21" s="95"/>
       <c r="K21" s="27"/>
       <c r="L21" s="27"/>
       <c r="M21" s="27"/>
@@ -2303,14 +2373,15 @@
       <c r="R21" s="27"/>
       <c r="S21" s="27"/>
       <c r="T21" s="27"/>
+      <c r="U21" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A3:W3"/>
-    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="A3:X3"/>
+    <mergeCell ref="A1:V1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="77" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2325,21 +2396,21 @@
       <selection activeCell="A3" sqref="A3:M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="5" width="8.42578125" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" customWidth="1"/>
+    <col min="3" max="5" width="8.453125" customWidth="1"/>
+    <col min="6" max="7" width="9.1796875" customWidth="1"/>
+    <col min="8" max="8" width="8.453125" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
-    <col min="11" max="12" width="8.42578125" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="8.42578125" customWidth="1"/>
+    <col min="11" max="12" width="8.453125" customWidth="1"/>
+    <col min="13" max="13" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="79" t="s">
         <v>16</v>
       </c>
@@ -2356,7 +2427,7 @@
       <c r="L1" s="80"/>
       <c r="M1" s="81"/>
     </row>
-    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="23"/>
       <c r="B2" s="22"/>
       <c r="C2" s="20"/>
@@ -2370,7 +2441,7 @@
       <c r="L2" s="19"/>
       <c r="M2" s="19"/>
     </row>
-    <row r="3" spans="1:17" s="61" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" s="61" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="78"/>
       <c r="B3" s="78"/>
       <c r="C3" s="78"/>
@@ -2385,7 +2456,7 @@
       <c r="L3" s="78"/>
       <c r="M3" s="78"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="59"/>
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
@@ -2400,7 +2471,7 @@
       <c r="L4" s="59"/>
       <c r="M4" s="59"/>
     </row>
-    <row r="5" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="14"/>
       <c r="B5" s="18"/>
       <c r="C5" s="14"/>
@@ -2415,7 +2486,7 @@
       <c r="L5" s="15"/>
       <c r="M5" s="14"/>
     </row>
-    <row r="6" spans="1:17" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="49" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="40" t="s">
         <v>30</v>
       </c>
@@ -2460,7 +2531,7 @@
       <c r="P6" s="13"/>
       <c r="Q6" s="13"/>
     </row>
-    <row r="7" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A7" s="60"/>
       <c r="B7" s="46">
         <v>12245</v>
@@ -2512,7 +2583,7 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>0</v>
       </c>
@@ -2536,7 +2607,7 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="10"/>
       <c r="C9" s="2"/>
@@ -2555,7 +2626,7 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="57"/>
       <c r="B10" s="58"/>
       <c r="C10" s="57"/>
@@ -2574,7 +2645,7 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="24"/>
       <c r="B11" s="24"/>
       <c r="C11" s="24"/>
@@ -2589,7 +2660,7 @@
       <c r="L11" s="24"/>
       <c r="M11" s="11"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
       <c r="B12" s="10"/>
       <c r="C12" s="6"/>
@@ -2608,7 +2679,7 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="6"/>
       <c r="B13" s="10"/>
       <c r="C13" s="6"/>
@@ -2627,7 +2698,7 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="6"/>
       <c r="B14" s="10"/>
       <c r="C14" s="6"/>
@@ -2646,7 +2717,7 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="24"/>
       <c r="B15" s="10"/>
       <c r="C15" s="6"/>
@@ -2665,7 +2736,7 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="6"/>
       <c r="B16" s="10"/>
       <c r="C16" s="6"/>
@@ -2684,7 +2755,7 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="26"/>
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
@@ -2698,7 +2769,7 @@
       <c r="K17" s="27"/>
       <c r="L17" s="27"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="26"/>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
@@ -2712,7 +2783,7 @@
       <c r="K18" s="27"/>
       <c r="L18" s="27"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="27"/>
       <c r="B19" s="27"/>
       <c r="C19" s="27"/>
@@ -2726,7 +2797,7 @@
       <c r="K19" s="27"/>
       <c r="L19" s="27"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="27"/>
       <c r="B20" s="27"/>
       <c r="C20" s="27"/>
@@ -2740,7 +2811,7 @@
       <c r="K20" s="27"/>
       <c r="L20" s="27"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="27"/>
       <c r="B21" s="27"/>
       <c r="C21" s="27"/>
@@ -2775,21 +2846,21 @@
       <selection activeCell="A3" sqref="A3:N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="6" width="8.42578125" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" customWidth="1"/>
+    <col min="3" max="6" width="8.453125" customWidth="1"/>
+    <col min="7" max="8" width="9.1796875" customWidth="1"/>
+    <col min="9" max="9" width="8.453125" customWidth="1"/>
     <col min="10" max="10" width="10" customWidth="1"/>
     <col min="11" max="11" width="9" customWidth="1"/>
-    <col min="12" max="13" width="8.42578125" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="8.42578125" customWidth="1"/>
+    <col min="12" max="13" width="8.453125" customWidth="1"/>
+    <col min="14" max="14" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:18" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="79" t="s">
         <v>16</v>
       </c>
@@ -2807,7 +2878,7 @@
       <c r="M1" s="80"/>
       <c r="N1" s="81"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="23"/>
       <c r="B2" s="22"/>
       <c r="C2" s="20"/>
@@ -2821,7 +2892,7 @@
       <c r="M2" s="19"/>
       <c r="N2" s="19"/>
     </row>
-    <row r="3" spans="1:18" s="61" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" s="61" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="78"/>
       <c r="B3" s="78"/>
       <c r="C3" s="78"/>
@@ -2837,7 +2908,7 @@
       <c r="M3" s="78"/>
       <c r="N3" s="78"/>
     </row>
-    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="59"/>
       <c r="B4" s="47"/>
       <c r="C4" s="47"/>
@@ -2853,7 +2924,7 @@
       <c r="M4" s="47"/>
       <c r="N4" s="47"/>
     </row>
-    <row r="5" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="14"/>
       <c r="B5" s="18"/>
       <c r="C5" s="14"/>
@@ -2869,7 +2940,7 @@
       <c r="M5" s="15"/>
       <c r="N5" s="14"/>
     </row>
-    <row r="6" spans="1:18" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="49" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="40" t="s">
         <v>30</v>
       </c>
@@ -2917,7 +2988,7 @@
       <c r="Q6" s="13"/>
       <c r="R6" s="13"/>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A7" s="60" t="s">
         <v>1</v>
       </c>
@@ -2974,7 +3045,7 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>0</v>
       </c>
@@ -2999,7 +3070,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="10"/>
       <c r="C9" s="2"/>
@@ -3019,7 +3090,7 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="6"/>
       <c r="B10" s="10"/>
       <c r="C10" s="6"/>
@@ -3039,7 +3110,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="24"/>
       <c r="B11" s="24"/>
       <c r="C11" s="24"/>
@@ -3055,7 +3126,7 @@
       <c r="M11" s="24"/>
       <c r="N11" s="11"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
       <c r="B12" s="10"/>
       <c r="C12" s="6"/>
@@ -3075,7 +3146,7 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="6"/>
       <c r="B13" s="10"/>
       <c r="C13" s="6"/>
@@ -3095,7 +3166,7 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="6"/>
       <c r="B14" s="10"/>
       <c r="C14" s="6"/>
@@ -3115,7 +3186,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" s="24"/>
       <c r="B15" s="10"/>
       <c r="C15" s="6"/>
@@ -3135,7 +3206,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" s="6"/>
       <c r="B16" s="10"/>
       <c r="C16" s="6"/>
@@ -3155,7 +3226,7 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="26"/>
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
@@ -3170,7 +3241,7 @@
       <c r="L17" s="27"/>
       <c r="M17" s="27"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="26"/>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
@@ -3185,7 +3256,7 @@
       <c r="L18" s="27"/>
       <c r="M18" s="27"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="27"/>
       <c r="B19" s="27"/>
       <c r="C19" s="27"/>
@@ -3200,7 +3271,7 @@
       <c r="L19" s="27"/>
       <c r="M19" s="27"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="27"/>
       <c r="B20" s="27"/>
       <c r="C20" s="27"/>
@@ -3215,7 +3286,7 @@
       <c r="L20" s="27"/>
       <c r="M20" s="27"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="27"/>
       <c r="B21" s="27"/>
       <c r="C21" s="27"/>
@@ -3251,22 +3322,22 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.7265625" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.54296875" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="13" width="15.5703125" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+    <col min="10" max="13" width="15.54296875" customWidth="1"/>
+    <col min="14" max="14" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" ht="24" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="84" t="s">
         <v>35</v>
       </c>
@@ -3284,11 +3355,11 @@
       <c r="M1" s="85"/>
       <c r="N1" s="86"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C2" s="56"/>
       <c r="D2" s="55"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="82"/>
       <c r="B3" s="82"/>
       <c r="C3" s="82"/>
@@ -3303,7 +3374,7 @@
       <c r="L3" s="72"/>
       <c r="M3" s="72"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="83"/>
       <c r="B4" s="83"/>
       <c r="C4" s="83"/>
@@ -3316,7 +3387,7 @@
       <c r="L4" s="53"/>
       <c r="M4" s="53"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="50"/>
       <c r="B5" s="50"/>
       <c r="C5" s="52"/>
@@ -3331,7 +3402,7 @@
       <c r="L5" s="50"/>
       <c r="M5" s="50"/>
     </row>
-    <row r="6" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="49" t="s">
         <v>30</v>
       </c>
@@ -3375,7 +3446,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="48" t="s">
         <v>20</v>
       </c>

</xml_diff>